<commit_message>
lengkapin data sep 11
</commit_message>
<xml_diff>
--- a/data_suhu/september/11-09-23-Lokasi2 (data semi rapih).xlsx
+++ b/data_suhu/september/11-09-23-Lokasi2 (data semi rapih).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josev\Downloads\magang_res\data_suhu\september\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josev\Downloads\magang_res_cloned\data_suhu\september\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16138DD2-40D7-4BAD-80B2-23435F4023F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4994F2C7-403D-4500-A394-53FA75D4BB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B56DACF4-C4E7-41AB-9AD1-37DA836393D6}"/>
+    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{B56DACF4-C4E7-41AB-9AD1-37DA836393D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -302,7 +302,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -372,7 +372,7 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF714EC-14B9-4D74-BDCF-754D8409DB8C}">
   <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>